<commit_message>
Update EPC data (combined, every-3-days)
</commit_message>
<xml_diff>
--- a/data/adtraction_epc_medians.xlsx
+++ b/data/adtraction_epc_medians.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +494,49 @@
         <is>
           <t>2025-10-22</t>
         </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-10-22</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>5.68</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9.32</v>
+      </c>
+      <c r="D3" t="n">
+        <v>7.66</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5.03</v>
+      </c>
+      <c r="F3" t="n">
+        <v>26.84</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="H3" t="n">
+        <v>5.36</v>
+      </c>
+      <c r="I3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="K3" t="n">
+        <v>12.58</v>
+      </c>
+      <c r="L3" t="n">
+        <v>5.83</v>
+      </c>
+      <c r="M3" t="n">
+        <v>5.68</v>
       </c>
     </row>
   </sheetData>
@@ -507,7 +550,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,6 +632,13 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-10-22</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>